<commit_message>
Graph And Computation for quicksort
</commit_message>
<xml_diff>
--- a/QuickSort.xlsx
+++ b/QuickSort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronit\Desktop\Git_Repo\Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A6A770-BABE-464D-AB21-F9D6B7FC41C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48863B77-F274-44A2-89E4-98D527CE2250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,7 +350,7 @@
                   <c:v>532400</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>759400</c:v>
+                  <c:v>759420</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>914900</c:v>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>759400</v>
+        <v>759420</v>
       </c>
       <c r="B16">
         <v>1522</v>

</xml_diff>